<commit_message>
Read in geographies, write to-do list
</commit_message>
<xml_diff>
--- a/Cook County Assessment Ratios.xlsx
+++ b/Cook County Assessment Ratios.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sawyer\Documents\Gov't Effectiveness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\midde\OneDrive\Documents\GitHub\IL-Gov-Counter\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E5FC41E-DCBD-401E-973E-58C285EB8F42}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21333" windowHeight="9280"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cook County Assessment Ratios" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="35">
   <si>
     <t>Year</t>
   </si>
@@ -134,7 +135,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -469,21 +470,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D331"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A345" workbookViewId="0">
+      <selection activeCell="F355" sqref="F355"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.9375" style="1"/>
-    <col min="2" max="4" width="25.64453125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.9375" style="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="4" width="25.6640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -497,7 +498,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2006</v>
       </c>
@@ -511,7 +512,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2006</v>
       </c>
@@ -525,7 +526,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2006</v>
       </c>
@@ -539,7 +540,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2006</v>
       </c>
@@ -553,7 +554,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2006</v>
       </c>
@@ -567,7 +568,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2006</v>
       </c>
@@ -581,7 +582,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
@@ -595,7 +596,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2006</v>
       </c>
@@ -609,7 +610,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2006</v>
       </c>
@@ -623,7 +624,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2006</v>
       </c>
@@ -637,7 +638,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2006</v>
       </c>
@@ -651,7 +652,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2006</v>
       </c>
@@ -665,7 +666,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2006</v>
       </c>
@@ -679,7 +680,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2006</v>
       </c>
@@ -693,7 +694,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2006</v>
       </c>
@@ -707,7 +708,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>2006</v>
       </c>
@@ -721,7 +722,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>2006</v>
       </c>
@@ -735,7 +736,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>2006</v>
       </c>
@@ -749,7 +750,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>2006</v>
       </c>
@@ -763,7 +764,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>2006</v>
       </c>
@@ -777,7 +778,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>2006</v>
       </c>
@@ -791,7 +792,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>2006</v>
       </c>
@@ -805,7 +806,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>2006</v>
       </c>
@@ -819,7 +820,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>2006</v>
       </c>
@@ -833,7 +834,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>2006</v>
       </c>
@@ -847,7 +848,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>2006</v>
       </c>
@@ -861,7 +862,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>2006</v>
       </c>
@@ -875,7 +876,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>2006</v>
       </c>
@@ -889,7 +890,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>2006</v>
       </c>
@@ -903,7 +904,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>2006</v>
       </c>
@@ -917,7 +918,7 @@
         <v>2.7075999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>2007</v>
       </c>
@@ -931,7 +932,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>2007</v>
       </c>
@@ -945,7 +946,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>2007</v>
       </c>
@@ -959,7 +960,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>2007</v>
       </c>
@@ -973,7 +974,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>2007</v>
       </c>
@@ -987,7 +988,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>2007</v>
       </c>
@@ -1001,7 +1002,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>2007</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>2007</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>2007</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>2007</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>2007</v>
       </c>
@@ -1071,7 +1072,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>2007</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>2007</v>
       </c>
@@ -1099,7 +1100,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>2007</v>
       </c>
@@ -1113,7 +1114,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>2007</v>
       </c>
@@ -1127,7 +1128,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>2007</v>
       </c>
@@ -1141,7 +1142,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>2007</v>
       </c>
@@ -1155,7 +1156,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>2007</v>
       </c>
@@ -1169,7 +1170,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>2007</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>2007</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>2007</v>
       </c>
@@ -1211,7 +1212,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>2007</v>
       </c>
@@ -1225,7 +1226,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>2007</v>
       </c>
@@ -1239,7 +1240,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>2007</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>2007</v>
       </c>
@@ -1267,7 +1268,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>2007</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>2007</v>
       </c>
@@ -1295,7 +1296,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>2007</v>
       </c>
@@ -1309,7 +1310,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>2007</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>2007</v>
       </c>
@@ -1337,7 +1338,7 @@
         <v>2.8439000000000001</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>2008</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>2008</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>2008</v>
       </c>
@@ -1379,7 +1380,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>2008</v>
       </c>
@@ -1393,7 +1394,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>2008</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>2008</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>2008</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>2008</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>2008</v>
       </c>
@@ -1463,7 +1464,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>2008</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>2008</v>
       </c>
@@ -1491,7 +1492,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>2008</v>
       </c>
@@ -1505,7 +1506,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>2008</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>2008</v>
       </c>
@@ -1533,7 +1534,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>2008</v>
       </c>
@@ -1547,7 +1548,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>2008</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>2008</v>
       </c>
@@ -1575,7 +1576,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>2008</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>2008</v>
       </c>
@@ -1603,7 +1604,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>2008</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>2008</v>
       </c>
@@ -1631,7 +1632,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>2008</v>
       </c>
@@ -1645,7 +1646,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>2008</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>2008</v>
       </c>
@@ -1673,7 +1674,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>2008</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>2008</v>
       </c>
@@ -1701,7 +1702,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>2008</v>
       </c>
@@ -1715,7 +1716,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>2008</v>
       </c>
@@ -1729,7 +1730,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>2008</v>
       </c>
@@ -1743,7 +1744,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>2008</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>2.9786000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>2009</v>
       </c>
@@ -1771,7 +1772,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>2009</v>
       </c>
@@ -1785,7 +1786,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>2009</v>
       </c>
@@ -1799,7 +1800,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>2009</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>2009</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>2009</v>
       </c>
@@ -1841,7 +1842,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>2009</v>
       </c>
@@ -1855,7 +1856,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>2009</v>
       </c>
@@ -1869,7 +1870,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>2009</v>
       </c>
@@ -1883,7 +1884,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>2009</v>
       </c>
@@ -1897,7 +1898,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>2009</v>
       </c>
@@ -1911,7 +1912,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>2009</v>
       </c>
@@ -1925,7 +1926,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>2009</v>
       </c>
@@ -1939,7 +1940,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>2009</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>2009</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>2009</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>2009</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>2009</v>
       </c>
@@ -2009,7 +2010,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>2009</v>
       </c>
@@ -2023,7 +2024,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>2009</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>2009</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>2009</v>
       </c>
@@ -2065,7 +2066,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>2009</v>
       </c>
@@ -2079,7 +2080,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>2009</v>
       </c>
@@ -2093,7 +2094,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>2009</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>2009</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>2009</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>2009</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>2009</v>
       </c>
@@ -2163,7 +2164,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>2009</v>
       </c>
@@ -2177,7 +2178,7 @@
         <v>3.3700999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>2010</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>2010</v>
       </c>
@@ -2205,7 +2206,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>2010</v>
       </c>
@@ -2219,7 +2220,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>2010</v>
       </c>
@@ -2233,7 +2234,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>2010</v>
       </c>
@@ -2247,7 +2248,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>2010</v>
       </c>
@@ -2261,7 +2262,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>2010</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>2010</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>2010</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>2010</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>2010</v>
       </c>
@@ -2331,7 +2332,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>2010</v>
       </c>
@@ -2345,7 +2346,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>2010</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>2010</v>
       </c>
@@ -2373,7 +2374,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>2010</v>
       </c>
@@ -2387,7 +2388,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>2010</v>
       </c>
@@ -2401,7 +2402,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>2010</v>
       </c>
@@ -2415,7 +2416,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>2010</v>
       </c>
@@ -2429,7 +2430,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>2010</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>2010</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>2010</v>
       </c>
@@ -2471,7 +2472,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>2010</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>2010</v>
       </c>
@@ -2499,7 +2500,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>2010</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>2010</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>2010</v>
       </c>
@@ -2541,7 +2542,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>2010</v>
       </c>
@@ -2555,7 +2556,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>2010</v>
       </c>
@@ -2569,7 +2570,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>2010</v>
       </c>
@@ -2583,7 +2584,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>2010</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>2011</v>
       </c>
@@ -2611,7 +2612,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>2011</v>
       </c>
@@ -2625,7 +2626,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>2011</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>2011</v>
       </c>
@@ -2653,7 +2654,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>2011</v>
       </c>
@@ -2667,7 +2668,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>2011</v>
       </c>
@@ -2681,7 +2682,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>2011</v>
       </c>
@@ -2695,7 +2696,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>2011</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>2011</v>
       </c>
@@ -2723,7 +2724,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>2011</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>2011</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>2011</v>
       </c>
@@ -2765,7 +2766,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>2011</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>2011</v>
       </c>
@@ -2793,7 +2794,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>2011</v>
       </c>
@@ -2807,7 +2808,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>2011</v>
       </c>
@@ -2821,7 +2822,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>2011</v>
       </c>
@@ -2835,7 +2836,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>2011</v>
       </c>
@@ -2849,7 +2850,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>2011</v>
       </c>
@@ -2863,7 +2864,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>2011</v>
       </c>
@@ -2877,7 +2878,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>2011</v>
       </c>
@@ -2891,7 +2892,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>2011</v>
       </c>
@@ -2905,7 +2906,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>2011</v>
       </c>
@@ -2919,7 +2920,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>2011</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>2011</v>
       </c>
@@ -2947,7 +2948,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>2011</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>2011</v>
       </c>
@@ -2975,7 +2976,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>2011</v>
       </c>
@@ -2989,7 +2990,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>2011</v>
       </c>
@@ -3003,7 +3004,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>2011</v>
       </c>
@@ -3017,7 +3018,7 @@
         <v>2.9706000000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>2012</v>
       </c>
@@ -3031,7 +3032,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>2012</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>2012</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>2012</v>
       </c>
@@ -3073,7 +3074,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>2012</v>
       </c>
@@ -3087,7 +3088,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>2012</v>
       </c>
@@ -3101,7 +3102,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>2012</v>
       </c>
@@ -3115,7 +3116,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>2012</v>
       </c>
@@ -3129,7 +3130,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>2012</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>2012</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>2012</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>2012</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>2012</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>2012</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>2012</v>
       </c>
@@ -3227,7 +3228,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>2012</v>
       </c>
@@ -3241,7 +3242,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>2012</v>
       </c>
@@ -3255,7 +3256,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>2012</v>
       </c>
@@ -3269,7 +3270,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>2012</v>
       </c>
@@ -3283,7 +3284,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>2012</v>
       </c>
@@ -3297,7 +3298,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>2012</v>
       </c>
@@ -3311,7 +3312,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>2012</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>2012</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>2012</v>
       </c>
@@ -3353,7 +3354,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>2012</v>
       </c>
@@ -3367,7 +3368,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>2012</v>
       </c>
@@ -3381,7 +3382,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>2012</v>
       </c>
@@ -3395,7 +3396,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>2012</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>2012</v>
       </c>
@@ -3423,7 +3424,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>2012</v>
       </c>
@@ -3437,7 +3438,7 @@
         <v>2.8056000000000001</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>2013</v>
       </c>
@@ -3451,7 +3452,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>2013</v>
       </c>
@@ -3465,7 +3466,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>2013</v>
       </c>
@@ -3479,7 +3480,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>2013</v>
       </c>
@@ -3493,7 +3494,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>2013</v>
       </c>
@@ -3507,7 +3508,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>2013</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>2013</v>
       </c>
@@ -3535,7 +3536,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>2013</v>
       </c>
@@ -3549,7 +3550,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>2013</v>
       </c>
@@ -3563,7 +3564,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>2013</v>
       </c>
@@ -3577,7 +3578,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>2013</v>
       </c>
@@ -3591,7 +3592,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>2013</v>
       </c>
@@ -3605,7 +3606,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>2013</v>
       </c>
@@ -3619,7 +3620,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>2013</v>
       </c>
@@ -3633,7 +3634,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>2013</v>
       </c>
@@ -3647,7 +3648,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>2013</v>
       </c>
@@ -3661,7 +3662,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>2013</v>
       </c>
@@ -3675,7 +3676,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>2013</v>
       </c>
@@ -3689,7 +3690,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>2013</v>
       </c>
@@ -3703,7 +3704,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>2013</v>
       </c>
@@ -3717,7 +3718,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>2013</v>
       </c>
@@ -3731,7 +3732,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>2013</v>
       </c>
@@ -3745,7 +3746,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>2013</v>
       </c>
@@ -3759,7 +3760,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>2013</v>
       </c>
@@ -3773,7 +3774,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>2013</v>
       </c>
@@ -3787,7 +3788,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>2013</v>
       </c>
@@ -3801,7 +3802,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>2013</v>
       </c>
@@ -3815,7 +3816,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>2013</v>
       </c>
@@ -3829,7 +3830,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>2013</v>
       </c>
@@ -3843,7 +3844,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>2013</v>
       </c>
@@ -3857,7 +3858,7 @@
         <v>2.6621000000000001</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>2014</v>
       </c>
@@ -3871,7 +3872,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>2014</v>
       </c>
@@ -3885,7 +3886,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>2014</v>
       </c>
@@ -3899,7 +3900,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>2014</v>
       </c>
@@ -3913,7 +3914,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>2014</v>
       </c>
@@ -3927,7 +3928,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>2014</v>
       </c>
@@ -3941,7 +3942,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>2014</v>
       </c>
@@ -3955,7 +3956,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>2014</v>
       </c>
@@ -3969,7 +3970,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>2014</v>
       </c>
@@ -3983,7 +3984,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>2014</v>
       </c>
@@ -3997,7 +3998,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>2014</v>
       </c>
@@ -4011,7 +4012,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253" s="1">
         <v>2014</v>
       </c>
@@ -4025,7 +4026,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254" s="1">
         <v>2014</v>
       </c>
@@ -4039,7 +4040,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255" s="1">
         <v>2014</v>
       </c>
@@ -4053,7 +4054,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256" s="1">
         <v>2014</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257" s="1">
         <v>2014</v>
       </c>
@@ -4081,7 +4082,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258" s="1">
         <v>2014</v>
       </c>
@@ -4095,7 +4096,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259" s="1">
         <v>2014</v>
       </c>
@@ -4109,7 +4110,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260" s="1">
         <v>2014</v>
       </c>
@@ -4123,7 +4124,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261" s="1">
         <v>2014</v>
       </c>
@@ -4137,7 +4138,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262" s="1">
         <v>2014</v>
       </c>
@@ -4151,7 +4152,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263" s="1">
         <v>2014</v>
       </c>
@@ -4165,7 +4166,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264" s="1">
         <v>2014</v>
       </c>
@@ -4179,7 +4180,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265" s="1">
         <v>2014</v>
       </c>
@@ -4193,7 +4194,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266" s="1">
         <v>2014</v>
       </c>
@@ -4207,7 +4208,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267" s="1">
         <v>2014</v>
       </c>
@@ -4221,7 +4222,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268" s="1">
         <v>2014</v>
       </c>
@@ -4235,7 +4236,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269" s="1">
         <v>2014</v>
       </c>
@@ -4249,7 +4250,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270" s="1">
         <v>2014</v>
       </c>
@@ -4263,7 +4264,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271" s="1">
         <v>2014</v>
       </c>
@@ -4277,7 +4278,7 @@
         <v>2.7252999999999998</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272" s="1">
         <v>2015</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273" s="1">
         <v>2015</v>
       </c>
@@ -4305,7 +4306,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274" s="1">
         <v>2015</v>
       </c>
@@ -4319,7 +4320,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275" s="1">
         <v>2015</v>
       </c>
@@ -4333,7 +4334,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276" s="1">
         <v>2015</v>
       </c>
@@ -4347,7 +4348,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277" s="1">
         <v>2015</v>
       </c>
@@ -4361,7 +4362,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278" s="1">
         <v>2015</v>
       </c>
@@ -4375,7 +4376,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279" s="1">
         <v>2015</v>
       </c>
@@ -4389,7 +4390,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280" s="1">
         <v>2015</v>
       </c>
@@ -4403,7 +4404,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281" s="1">
         <v>2015</v>
       </c>
@@ -4417,7 +4418,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282" s="1">
         <v>2015</v>
       </c>
@@ -4431,7 +4432,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283" s="1">
         <v>2015</v>
       </c>
@@ -4445,7 +4446,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284" s="1">
         <v>2015</v>
       </c>
@@ -4459,7 +4460,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285" s="1">
         <v>2015</v>
       </c>
@@ -4473,7 +4474,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286" s="1">
         <v>2015</v>
       </c>
@@ -4487,7 +4488,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287" s="1">
         <v>2015</v>
       </c>
@@ -4501,7 +4502,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288" s="1">
         <v>2015</v>
       </c>
@@ -4515,7 +4516,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289" s="1">
         <v>2015</v>
       </c>
@@ -4529,7 +4530,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290" s="1">
         <v>2015</v>
       </c>
@@ -4543,7 +4544,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291" s="1">
         <v>2015</v>
       </c>
@@ -4557,7 +4558,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292" s="1">
         <v>2015</v>
       </c>
@@ -4571,7 +4572,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293" s="1">
         <v>2015</v>
       </c>
@@ -4585,7 +4586,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294" s="1">
         <v>2015</v>
       </c>
@@ -4599,7 +4600,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295" s="1">
         <v>2015</v>
       </c>
@@ -4613,7 +4614,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296" s="1">
         <v>2015</v>
       </c>
@@ -4627,7 +4628,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297" s="1">
         <v>2015</v>
       </c>
@@ -4641,7 +4642,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298" s="1">
         <v>2015</v>
       </c>
@@ -4655,7 +4656,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299" s="1">
         <v>2015</v>
       </c>
@@ -4669,7 +4670,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300" s="1">
         <v>2015</v>
       </c>
@@ -4683,7 +4684,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301" s="1">
         <v>2015</v>
       </c>
@@ -4697,7 +4698,7 @@
         <v>2.6684999999999999</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302" s="1">
         <v>2016</v>
       </c>
@@ -4711,7 +4712,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303" s="1">
         <v>2016</v>
       </c>
@@ -4725,7 +4726,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304" s="1">
         <v>2016</v>
       </c>
@@ -4739,7 +4740,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305" s="1">
         <v>2016</v>
       </c>
@@ -4753,7 +4754,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306" s="1">
         <v>2016</v>
       </c>
@@ -4767,7 +4768,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307" s="1">
         <v>2016</v>
       </c>
@@ -4781,7 +4782,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308" s="1">
         <v>2016</v>
       </c>
@@ -4795,7 +4796,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309" s="1">
         <v>2016</v>
       </c>
@@ -4809,7 +4810,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310" s="1">
         <v>2016</v>
       </c>
@@ -4823,7 +4824,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311" s="1">
         <v>2016</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312" s="1">
         <v>2016</v>
       </c>
@@ -4851,7 +4852,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313" s="1">
         <v>2016</v>
       </c>
@@ -4865,7 +4866,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314" s="1">
         <v>2016</v>
       </c>
@@ -4879,7 +4880,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315" s="1">
         <v>2016</v>
       </c>
@@ -4893,7 +4894,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316" s="1">
         <v>2016</v>
       </c>
@@ -4907,7 +4908,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317" s="1">
         <v>2016</v>
       </c>
@@ -4921,7 +4922,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318" s="1">
         <v>2016</v>
       </c>
@@ -4935,7 +4936,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319" s="1">
         <v>2016</v>
       </c>
@@ -4949,7 +4950,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320" s="1">
         <v>2016</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321" s="1">
         <v>2016</v>
       </c>
@@ -4977,7 +4978,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322" s="1">
         <v>2016</v>
       </c>
@@ -4991,7 +4992,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323" s="1">
         <v>2016</v>
       </c>
@@ -5005,7 +5006,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324" s="1">
         <v>2016</v>
       </c>
@@ -5019,7 +5020,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325" s="1">
         <v>2016</v>
       </c>
@@ -5033,7 +5034,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="326" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A326" s="1">
         <v>2016</v>
       </c>
@@ -5047,7 +5048,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="327" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A327" s="1">
         <v>2016</v>
       </c>
@@ -5061,7 +5062,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="328" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A328" s="1">
         <v>2016</v>
       </c>
@@ -5075,7 +5076,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="329" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A329" s="1">
         <v>2016</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="330" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A330" s="1">
         <v>2016</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>2.8031999999999999</v>
       </c>
     </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A331" s="1">
         <v>2016</v>
       </c>
@@ -5115,6 +5116,426 @@
       </c>
       <c r="D331" s="1">
         <v>2.8031999999999999</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A332" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C332" s="1">
+        <v>10.220000000000001</v>
+      </c>
+      <c r="D332" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A333" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B333" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C333" s="1">
+        <v>9.0299999999999994</v>
+      </c>
+      <c r="D333" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A334" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C334" s="1">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="D334" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A335" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B335" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C335" s="1">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="D335" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A336" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C336" s="1">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="D336" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A337" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B337" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C337" s="1">
+        <v>8.44</v>
+      </c>
+      <c r="D337" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A338" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C338" s="1">
+        <v>9.07</v>
+      </c>
+      <c r="D338" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A339" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B339" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C339" s="1">
+        <v>8.83</v>
+      </c>
+      <c r="D339" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A340" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C340" s="1">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="D340" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A341" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B341" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C341" s="1">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="D341" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A342" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C342" s="1">
+        <v>9.27</v>
+      </c>
+      <c r="D342" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A343" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B343" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C343" s="1">
+        <v>8.93</v>
+      </c>
+      <c r="D343" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A344" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C344" s="1">
+        <v>8.64</v>
+      </c>
+      <c r="D344" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A345" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B345" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C345" s="1">
+        <v>7.05</v>
+      </c>
+      <c r="D345" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A346" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C346" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="D346" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A347" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B347" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C347" s="1">
+        <v>8.94</v>
+      </c>
+      <c r="D347" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A348" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C348" s="1">
+        <v>9.25</v>
+      </c>
+      <c r="D348" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A349" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C349" s="1">
+        <v>6.68</v>
+      </c>
+      <c r="D349" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A350" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C350" s="1">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="D350" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A351" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C351" s="1">
+        <v>7.96</v>
+      </c>
+      <c r="D351" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A352" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C352" s="1">
+        <v>7.74</v>
+      </c>
+      <c r="D352" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A353" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C353" s="1">
+        <v>8.69</v>
+      </c>
+      <c r="D353" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A354" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C354" s="1">
+        <v>8.56</v>
+      </c>
+      <c r="D354" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A355" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C355" s="1">
+        <v>7.76</v>
+      </c>
+      <c r="D355" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A356" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C356" s="1">
+        <v>9.44</v>
+      </c>
+      <c r="D356" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A357" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C357" s="1">
+        <v>7.58</v>
+      </c>
+      <c r="D357" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A358" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C358" s="1">
+        <v>7.69</v>
+      </c>
+      <c r="D358" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A359" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B359" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C359" s="1">
+        <v>8.08</v>
+      </c>
+      <c r="D359" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A360" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C360" s="1">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="D360" s="1">
+        <v>2.9626999999999999</v>
+      </c>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A361" s="1">
+        <v>2017</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C361" s="1">
+        <v>8.81</v>
+      </c>
+      <c r="D361" s="1">
+        <v>2.9626999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>